<commit_message>
Update Venture Valuation Tool by Foresight.xlsx
</commit_message>
<xml_diff>
--- a/Venture Valuation Tool by Foresight.xlsx
+++ b/Venture Valuation Tool by Foresight.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/taylordavidson/Documents/dev/cap-table-tool/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AAFD6463-ABC3-7F4D-87C4-3DAA4762F0C0}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{16242575-EC1C-144D-A662-2C697D0DE006}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="17540" xr2:uid="{509D9F61-49D3-DB4D-9E03-EA4CE0D5BC09}"/>
   </bookViews>
@@ -21,7 +21,7 @@
   <definedNames>
     <definedName name="_xlnm.Print_Area" localSheetId="0">README!$B$2:$B$33</definedName>
   </definedNames>
-  <calcPr calcId="191029" iterateCount="1000" iterateDelta="0.01"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -559,7 +559,7 @@
     <numFmt numFmtId="169" formatCode="_(* #,##0.000_);_(* \(#,##0.000\);_(* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="170" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
   </numFmts>
-  <fonts count="10">
+  <fonts count="11">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -618,8 +618,14 @@
       <color rgb="FF000000"/>
       <name val="Open Sans Regular"/>
     </font>
+    <font>
+      <sz val="14"/>
+      <color theme="1"/>
+      <name val="Avenir Book"/>
+      <family val="2"/>
+    </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -629,6 +635,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="0" tint="-4.9989318521683403E-2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFD9E1F3"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -651,7 +663,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="10">
+  <cellStyleXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -662,8 +674,9 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="70">
+  <cellXfs count="71">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -767,46 +780,47 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="8" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="6" applyFont="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="7" applyFont="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="6" applyFont="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="6" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="3" borderId="0" xfId="10" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="6" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="7" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="6" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="6" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="8" applyFont="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="8" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
       <alignment wrapText="1"/>
       <protection hidden="1"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="8" applyFont="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="9" fillId="3" borderId="0" xfId="8" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
       <alignment wrapText="1"/>
       <protection hidden="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="7" applyFont="1" applyAlignment="1">
-      <alignment wrapText="1"/>
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="0" xfId="7" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="0" xfId="7" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="7" applyFont="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="7" applyFont="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="6" applyFont="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="6" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
       <alignment wrapText="1"/>
       <protection hidden="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="7" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="7" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="7" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="0" xfId="7" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="7" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="7" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="7" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="7" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="7" applyFont="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="7" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="7" applyFont="1" applyFill="1"/>
   </cellXfs>
-  <cellStyles count="10">
+  <cellStyles count="11">
     <cellStyle name="Comma 10" xfId="3" xr:uid="{7E780D42-8F46-7445-8F61-6B969E5AD5E5}"/>
     <cellStyle name="Comma 17 2 2 2" xfId="1" xr:uid="{FE475603-AFFD-C548-9E28-5332CA5ECE32}"/>
     <cellStyle name="Comma 2" xfId="5" xr:uid="{953A3C49-DA33-354D-8447-C1C2AE0FF013}"/>
@@ -815,11 +829,17 @@
     <cellStyle name="Normal 8 2" xfId="6" xr:uid="{BD6D875F-DF14-3E4F-BC74-C4EA7C201A69}"/>
     <cellStyle name="Normal 8 2 2 3" xfId="9" xr:uid="{05ED5751-CFBF-F442-97EB-E4B2E04ED737}"/>
     <cellStyle name="Normal 8 2 3" xfId="7" xr:uid="{436B8513-AD05-DC42-971C-BBDC00583D1C}"/>
+    <cellStyle name="Normal 8 2 3 4" xfId="10" xr:uid="{430DD9A8-B4B3-1B46-9A48-85384810EA26}"/>
     <cellStyle name="Percent 10" xfId="4" xr:uid="{C9F276A3-4A7E-A441-83AF-EA921483D81B}"/>
     <cellStyle name="Percent 14 2 2 2" xfId="2" xr:uid="{909675B6-38E9-2E4C-B6F1-CD6B0A68A798}"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <colors>
+    <mruColors>
+      <color rgb="FFD9E1F3"/>
+    </mruColors>
+  </colors>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -832,100 +852,6 @@
 </file>
 
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>0</xdr:col>
-      <xdr:colOff>25400</xdr:colOff>
-      <xdr:row>0</xdr:row>
-      <xdr:rowOff>25400</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>3</xdr:col>
-      <xdr:colOff>3962400</xdr:colOff>
-      <xdr:row>18</xdr:row>
-      <xdr:rowOff>127000</xdr:rowOff>
-    </xdr:to>
-    <xdr:sp macro="" textlink="">
-      <xdr:nvSpPr>
-        <xdr:cNvPr id="2" name="Right Triangle 1">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{DA50F7B2-4475-F84E-8E74-78879E01FBAA}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvSpPr/>
-      </xdr:nvSpPr>
-      <xdr:spPr>
-        <a:xfrm flipV="1">
-          <a:off x="25400" y="25400"/>
-          <a:ext cx="10718800" cy="6870700"/>
-        </a:xfrm>
-        <a:prstGeom prst="rtTriangle">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:gradFill flip="none" rotWithShape="1">
-          <a:gsLst>
-            <a:gs pos="0">
-              <a:schemeClr val="accent1">
-                <a:tint val="100000"/>
-                <a:shade val="100000"/>
-                <a:satMod val="130000"/>
-                <a:alpha val="8000"/>
-              </a:schemeClr>
-            </a:gs>
-            <a:gs pos="100000">
-              <a:schemeClr val="accent1">
-                <a:tint val="50000"/>
-                <a:shade val="100000"/>
-                <a:satMod val="350000"/>
-                <a:alpha val="8000"/>
-              </a:schemeClr>
-            </a:gs>
-          </a:gsLst>
-          <a:lin ang="16200000" scaled="0"/>
-          <a:tileRect/>
-        </a:gradFill>
-        <a:ln>
-          <a:solidFill>
-            <a:schemeClr val="accent1">
-              <a:shade val="95000"/>
-              <a:satMod val="105000"/>
-              <a:alpha val="16000"/>
-            </a:schemeClr>
-          </a:solidFill>
-        </a:ln>
-      </xdr:spPr>
-      <xdr:style>
-        <a:lnRef idx="1">
-          <a:schemeClr val="accent1"/>
-        </a:lnRef>
-        <a:fillRef idx="3">
-          <a:schemeClr val="accent1"/>
-        </a:fillRef>
-        <a:effectRef idx="2">
-          <a:schemeClr val="accent1"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="lt1"/>
-        </a:fontRef>
-      </xdr:style>
-      <xdr:txBody>
-        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr algn="l"/>
-          <a:endParaRPr lang="en-US" sz="1100"/>
-        </a:p>
-      </xdr:txBody>
-    </xdr:sp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-</xdr:wsDr>
-</file>
-
-<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
@@ -1586,67 +1512,70 @@
   </sheetPr>
   <dimension ref="B2:D38"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0"/>
+    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+      <selection activeCell="D10" sqref="D10"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="21"/>
   <cols>
-    <col min="1" max="1" width="6.33203125" style="56" customWidth="1"/>
-    <col min="2" max="2" width="67.1640625" style="56" customWidth="1"/>
-    <col min="3" max="3" width="15.5" style="56" customWidth="1"/>
-    <col min="4" max="4" width="64.6640625" style="56" customWidth="1"/>
-    <col min="5" max="16384" width="9" style="56"/>
+    <col min="1" max="1" width="6.33203125" style="57" customWidth="1"/>
+    <col min="2" max="2" width="67.1640625" style="57" customWidth="1"/>
+    <col min="3" max="3" width="15.5" style="57" customWidth="1"/>
+    <col min="4" max="4" width="64.6640625" style="57" customWidth="1"/>
+    <col min="5" max="16384" width="9" style="57"/>
   </cols>
   <sheetData>
     <row r="2" spans="2:4">
-      <c r="B2" s="55" t="str">
+      <c r="B2" s="56" t="str">
         <f>UPPER(B25)&amp;" "&amp;UPPER(B26)&amp;" "&amp;UPPER(B27)&amp;" "&amp;IF(ISBLANK(B28),""," FOR "&amp;UPPER(B28))</f>
         <v xml:space="preserve">VENTURE VALUATION TOOL </v>
       </c>
-      <c r="C2" s="55"/>
+      <c r="C2" s="56"/>
     </row>
     <row r="3" spans="2:4">
-      <c r="B3" s="57"/>
-      <c r="C3" s="57"/>
+      <c r="B3" s="58"/>
+      <c r="C3" s="58"/>
     </row>
     <row r="4" spans="2:4" ht="22">
-      <c r="B4" s="58" t="s">
+      <c r="B4" s="59" t="s">
         <v>124</v>
       </c>
-      <c r="C4" s="58"/>
+      <c r="C4" s="59"/>
+      <c r="D4" s="55"/>
     </row>
     <row r="5" spans="2:4" ht="22">
-      <c r="B5" s="58" t="str">
+      <c r="B5" s="59" t="str">
         <f>"See more models at "&amp;"https://"&amp;B29</f>
         <v>See more models at https://foresight.is</v>
       </c>
-      <c r="C5" s="58"/>
+      <c r="C5" s="59"/>
     </row>
     <row r="6" spans="2:4" ht="22">
-      <c r="B6" s="58" t="str">
+      <c r="B6" s="59" t="str">
         <f>B30&amp;"@"&amp;B29&amp;" - @tdavidson"</f>
         <v>hello@foresight.is - @tdavidson</v>
       </c>
-      <c r="C6" s="58"/>
+      <c r="C6" s="59"/>
     </row>
     <row r="7" spans="2:4" ht="22">
-      <c r="B7" s="59" t="str">
+      <c r="B7" s="60" t="str">
         <f>"Questions, comments, ideas, email "&amp;B30&amp;"@"&amp;B29</f>
         <v>Questions, comments, ideas, email hello@foresight.is</v>
       </c>
-      <c r="C7" s="59"/>
+      <c r="C7" s="60"/>
     </row>
     <row r="8" spans="2:4" ht="22">
-      <c r="B8" s="60" t="s">
+      <c r="B8" s="61" t="s">
         <v>131</v>
       </c>
-      <c r="C8" s="60"/>
+      <c r="C8" s="61"/>
     </row>
     <row r="10" spans="2:4" ht="22" customHeight="1"/>
     <row r="11" spans="2:4" ht="22" customHeight="1">
-      <c r="B11" s="69" t="s">
+      <c r="B11" s="62" t="s">
         <v>166</v>
       </c>
-      <c r="D11" s="68" t="s">
+      <c r="D11" s="63" t="s">
         <v>167</v>
       </c>
     </row>
@@ -1660,7 +1589,7 @@
       </c>
     </row>
     <row r="13" spans="2:4" ht="22" customHeight="1">
-      <c r="B13" s="59" t="s">
+      <c r="B13" s="60" t="s">
         <v>156</v>
       </c>
       <c r="D13" s="65" t="str">
@@ -1669,18 +1598,18 @@
       </c>
     </row>
     <row r="14" spans="2:4">
-      <c r="B14" s="58"/>
-      <c r="C14" s="58"/>
+      <c r="B14" s="59"/>
+      <c r="C14" s="59"/>
     </row>
     <row r="15" spans="2:4">
-      <c r="B15" s="58"/>
-      <c r="C15" s="58"/>
+      <c r="B15" s="59"/>
+      <c r="C15" s="59"/>
     </row>
     <row r="16" spans="2:4" ht="22">
       <c r="B16" s="66" t="s">
         <v>125</v>
       </c>
-      <c r="C16" s="61"/>
+      <c r="C16" s="67"/>
       <c r="D16" s="66" t="s">
         <v>127</v>
       </c>
@@ -1689,21 +1618,21 @@
       <c r="B17" s="65" t="s">
         <v>126</v>
       </c>
-      <c r="C17" s="62"/>
+      <c r="C17" s="68"/>
       <c r="D17" s="65" t="s">
         <v>128</v>
       </c>
     </row>
     <row r="18" spans="2:4" ht="22" customHeight="1">
       <c r="B18" s="65"/>
-      <c r="C18" s="62"/>
+      <c r="C18" s="68"/>
       <c r="D18" s="65"/>
     </row>
     <row r="19" spans="2:4" ht="22">
       <c r="B19" s="66" t="s">
         <v>130</v>
       </c>
-      <c r="C19" s="62"/>
+      <c r="C19" s="68"/>
       <c r="D19" s="66" t="s">
         <v>129</v>
       </c>
@@ -1712,7 +1641,7 @@
       <c r="B20" s="65" t="s">
         <v>161</v>
       </c>
-      <c r="C20" s="61"/>
+      <c r="C20" s="67"/>
       <c r="D20" s="65" t="str">
         <f>"Visit https://"&amp;B29&amp;"/start to get more instructions and videos on how to use the model, including details on each sheet and key components."</f>
         <v>Visit https://foresight.is/start to get more instructions and videos on how to use the model, including details on each sheet and key components.</v>
@@ -1722,78 +1651,77 @@
       <c r="B21" s="65" t="s">
         <v>162</v>
       </c>
-      <c r="C21" s="62"/>
+      <c r="C21" s="68"/>
     </row>
     <row r="22" spans="2:4" ht="132">
       <c r="B22" s="65" t="s">
         <v>163</v>
       </c>
-      <c r="C22" s="61"/>
-      <c r="D22" s="61"/>
+      <c r="C22" s="67"/>
+      <c r="D22" s="67"/>
     </row>
     <row r="23" spans="2:4" ht="64" customHeight="1">
-      <c r="C23" s="62"/>
-      <c r="D23" s="67"/>
+      <c r="C23" s="68"/>
+      <c r="D23" s="69"/>
     </row>
     <row r="24" spans="2:4">
-      <c r="B24" s="63" t="s">
+      <c r="B24" s="70" t="s">
         <v>133</v>
       </c>
-      <c r="C24" s="62"/>
+      <c r="C24" s="68"/>
     </row>
     <row r="25" spans="2:4">
-      <c r="B25" s="56" t="s">
+      <c r="B25" s="57" t="s">
         <v>159</v>
       </c>
-      <c r="C25" s="62"/>
+      <c r="C25" s="68"/>
     </row>
     <row r="26" spans="2:4">
-      <c r="B26" s="56" t="s">
+      <c r="B26" s="57" t="s">
         <v>160</v>
       </c>
-      <c r="C26" s="62"/>
+      <c r="C26" s="68"/>
     </row>
     <row r="27" spans="2:4">
-      <c r="B27" s="56" t="s">
+      <c r="B27" s="57" t="s">
         <v>157</v>
       </c>
-      <c r="C27" s="62"/>
+      <c r="C27" s="68"/>
     </row>
     <row r="28" spans="2:4">
-      <c r="C28" s="62"/>
+      <c r="C28" s="68"/>
     </row>
     <row r="29" spans="2:4" ht="22">
-      <c r="B29" s="62" t="s">
+      <c r="B29" s="68" t="s">
         <v>164</v>
       </c>
-      <c r="C29" s="62"/>
+      <c r="C29" s="68"/>
     </row>
     <row r="30" spans="2:4" ht="22">
-      <c r="B30" s="62" t="s">
+      <c r="B30" s="68" t="s">
         <v>165</v>
       </c>
-      <c r="C30" s="62"/>
+      <c r="C30" s="68"/>
     </row>
     <row r="31" spans="2:4">
-      <c r="C31" s="61"/>
+      <c r="C31" s="67"/>
     </row>
     <row r="32" spans="2:4">
-      <c r="C32" s="62"/>
+      <c r="C32" s="68"/>
     </row>
     <row r="33" spans="2:3">
-      <c r="B33" s="61"/>
-      <c r="C33" s="61"/>
+      <c r="B33" s="67"/>
+      <c r="C33" s="67"/>
     </row>
     <row r="35" spans="2:3">
-      <c r="C35" s="63"/>
+      <c r="C35" s="70"/>
     </row>
     <row r="38" spans="2:3">
-      <c r="C38" s="63"/>
+      <c r="C38" s="70"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup scale="63" orientation="landscape" horizontalDpi="4294967292" verticalDpi="4294967292"/>
-  <drawing r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -7784,7 +7712,7 @@
     <sheetView showGridLines="0" workbookViewId="0">
       <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="B9" sqref="B9"/>
-      <selection pane="bottomLeft" activeCell="B9" sqref="B9"/>
+      <selection pane="bottomLeft" activeCell="B26" sqref="B26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="21"/>

</xml_diff>